<commit_message>
finished second set of graphs
</commit_message>
<xml_diff>
--- a/RO/FinalResultsGraphing/RO_Worksheet.xlsx
+++ b/RO/FinalResultsGraphing/RO_Worksheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steven/Desktop/5_CHEE_301B/CHEE_301B_Repo/RO/FinalResultsGraphing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27B135E-AE99-E448-825B-04F528AA453D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0223951A-35BA-0B46-BBDA-B47BE5421D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19480" activeTab="1" xr2:uid="{81BDDA59-F480-4C30-8BBC-AD1E6993C18D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19480" activeTab="2" xr2:uid="{81BDDA59-F480-4C30-8BBC-AD1E6993C18D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="fluxVsPressure" sheetId="3" r:id="rId2"/>
-    <sheet name="water density" sheetId="2" r:id="rId3"/>
+    <sheet name="fluxVsPDiff" sheetId="4" r:id="rId3"/>
+    <sheet name="water density" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Week 1</t>
   </si>
@@ -578,6 +579,15 @@
   </si>
   <si>
     <t>Run</t>
+  </si>
+  <si>
+    <t>Feed Osmotic pressure, pf (kPa)</t>
+  </si>
+  <si>
+    <t>Osmotic Pressure Difference (kPa)</t>
+  </si>
+  <si>
+    <t>Delta P - Delta Pi (kPa)</t>
   </si>
 </sst>
 </file>
@@ -3683,8 +3693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FF4BF0-FC9E-1649-B74A-1D2D26E94D1A}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:E13"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3949,6 +3959,505 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BAB2749-D02D-4E4E-8932-C02A790ACEB4}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="7" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="26" t="str" cm="1">
+        <f t="array" ref="B1:B13">TRANSPOSE(Sheet1!B13:N13)</f>
+        <v>Transmembrane Pressure drop, psi</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="26" t="str" cm="1">
+        <f t="array" ref="D1:D13">TRANSPOSE(Sheet1!B24:N24)</f>
+        <v>Feed Osmotic pressure, pf (atm)</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="26" t="str" cm="1">
+        <f t="array" ref="F1:F13">TRANSPOSE(Sheet1!B23:N23)</f>
+        <v>Permeate Osmotic pressure, pp (atm)</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="str" cm="1">
+        <f t="array" ref="J1:J13">fluxVsPressure!E1:E13</f>
+        <v>Water Flux corrected to 25°C Jw, L/m^2-hr</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <f>B2*6894.7572931783/1000</f>
+        <v>517.10679698837248</v>
+      </c>
+      <c r="D2">
+        <v>0.91451975007494879</v>
+      </c>
+      <c r="E2">
+        <f>D2*101.325</f>
+        <v>92.663713676344187</v>
+      </c>
+      <c r="F2">
+        <v>4.3589832215199346E-2</v>
+      </c>
+      <c r="G2">
+        <f>F2*101.325</f>
+        <v>4.4167397492050737</v>
+      </c>
+      <c r="H2">
+        <f>E2-G2</f>
+        <v>88.246973927139109</v>
+      </c>
+      <c r="I2">
+        <f>C2-H2</f>
+        <v>428.85982306123339</v>
+      </c>
+      <c r="J2">
+        <v>32.007555843285857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>115</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="0">B3*6894.7572931783/1000</f>
+        <v>792.89708871550454</v>
+      </c>
+      <c r="D3">
+        <v>0.91627883262645449</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E13" si="1">D3*101.325</f>
+        <v>92.841952715875507</v>
+      </c>
+      <c r="F3">
+        <v>3.8223213164998292E-2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G13" si="2">F3*101.325</f>
+        <v>3.8729670739434519</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H13" si="3">E3-G3</f>
+        <v>88.968985641932051</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I13" si="4">C3-H3</f>
+        <v>703.92810307357252</v>
+      </c>
+      <c r="J3">
+        <v>47.184464876331674</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>155</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1068.6873804426366</v>
+      </c>
+      <c r="D4">
+        <v>0.92476680694413071</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>93.701996713614051</v>
+      </c>
+      <c r="F4">
+        <v>3.0511134773485625E-2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>3.0915407309234308</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>90.610455982690624</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>978.07692445994599</v>
+      </c>
+      <c r="J4">
+        <v>62.432870639408186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>517.10679698837248</v>
+      </c>
+      <c r="D5">
+        <v>4.2109824011088293</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>426.67779179235214</v>
+      </c>
+      <c r="F5">
+        <v>0.44929767100231</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>45.525086514309059</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>381.15270527804307</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>135.95409171032941</v>
+      </c>
+      <c r="J5">
+        <v>12.620574924262856</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>115</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>792.89708871550454</v>
+      </c>
+      <c r="D6">
+        <v>4.1903821160831622</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>424.59046791212643</v>
+      </c>
+      <c r="F6">
+        <v>0.34255532228567753</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>34.709418030596275</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>389.88104988153015</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>403.01603883397439</v>
+      </c>
+      <c r="J6">
+        <v>28.194751638419142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>155</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1068.6873804426366</v>
+      </c>
+      <c r="D7">
+        <v>4.1839889241786441</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>423.94267774240114</v>
+      </c>
+      <c r="F7">
+        <v>0.24308459051805273</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>24.630546134241694</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>399.31213160815946</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>669.37524883447713</v>
+      </c>
+      <c r="J7">
+        <v>43.365814967433018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>517.10679698837248</v>
+      </c>
+      <c r="D8">
+        <v>0.80920338778151046</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>81.992533266961544</v>
+      </c>
+      <c r="F8">
+        <v>4.9033799046111368E-2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>4.9683496883472342</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>77.024183578614313</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>440.08261340975815</v>
+      </c>
+      <c r="J8">
+        <v>29.894976097153702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>115</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>792.89708871550454</v>
+      </c>
+      <c r="D9">
+        <v>0.81528969821107855</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>82.609228671237531</v>
+      </c>
+      <c r="F9">
+        <v>4.2777310196143309E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>4.3344109556242207</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>78.27481771561331</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>714.62227099989127</v>
+      </c>
+      <c r="J9">
+        <v>43.600417043516835</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>155</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>1068.6873804426366</v>
+      </c>
+      <c r="D10">
+        <v>0.81664666127516772</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>82.746722953706367</v>
+      </c>
+      <c r="F10">
+        <v>3.6449517883954279E-2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>3.6932473995916673</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>79.053475554114698</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>989.6339048885219</v>
+      </c>
+      <c r="J10">
+        <v>55.045895736950598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>75</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>517.10679698837248</v>
+      </c>
+      <c r="D11">
+        <v>3.5973435883873721</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>364.50083909335046</v>
+      </c>
+      <c r="F11">
+        <v>0.29583004684437864</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>29.974979496506666</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>334.52585959684382</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>182.58093739152866</v>
+      </c>
+      <c r="J11">
+        <v>14.546005889762828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>115</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>792.89708871550454</v>
+      </c>
+      <c r="D12">
+        <v>3.5946673041166464</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>364.22966458961918</v>
+      </c>
+      <c r="F12">
+        <v>0.21060640769917258</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>21.339694260118662</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>342.8899703295005</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>450.00711838600404</v>
+      </c>
+      <c r="J12">
+        <v>25.974021374800309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>155</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1068.6873804426366</v>
+      </c>
+      <c r="D13">
+        <v>3.6035882349453527</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>365.13357790583785</v>
+      </c>
+      <c r="F13">
+        <v>0.15335704463683825</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>15.538902547827636</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>349.59467535801019</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>719.09270508462646</v>
+      </c>
+      <c r="J13">
+        <v>40.319699452138998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD34794-4739-471C-8187-5C37806194C4}">
   <dimension ref="D4:H9"/>
   <sheetViews>

</xml_diff>